<commit_message>
Adding test cases for creating bike and dock
</commit_message>
<xml_diff>
--- a/unit_test/ecobike_testcase_specs.xlsx
+++ b/unit_test/ecobike_testcase_specs.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BKHN\Chous_Projects\ITTSS_Software_Development\ISD.ICT.20211-06\unit_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157E822B-3206-4080-A172-770E0BAE81D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F78F232-6305-4A1A-BFCD-21BBAFA8EAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{02D37FB5-232B-421C-A192-72757C7E38DB}"/>
   </bookViews>
   <sheets>
-    <sheet name="RentBikeServiceController" sheetId="1" r:id="rId1"/>
+    <sheet name="Bike" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>#</t>
   </si>
@@ -48,10 +48,60 @@
     <t>TEST CASE SPECIFICATIONS FOR ECOBIKE</t>
   </si>
   <si>
-    <t xml:space="preserve">Method name: </t>
-  </si>
-  <si>
     <t>Method name:</t>
+  </si>
+  <si>
+    <t>Method name: Bike (Constructor)</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>bike type</t>
+  </si>
+  <si>
+    <t>bike image</t>
+  </si>
+  <si>
+    <t>bike barcode</t>
+  </si>
+  <si>
+    <t>bike rental price</t>
+  </si>
+  <si>
+    <t>deposit price</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>create date</t>
+  </si>
+  <si>
+    <t>total rental time</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>battery</t>
+  </si>
+  <si>
+    <t>- must not be null or empty
+- must start with a letter
+- can only contain letters, number, space, dash - and underscore _</t>
+  </si>
+  <si>
+    <t>- must greater than 0</t>
+  </si>
+  <si>
+    <t>- must of 3 letter, abbreviation</t>
+  </si>
+  <si>
+    <t>- can only be FREE or RENTED</t>
+  </si>
+  <si>
+    <t>- must be in range 0 - 100</t>
   </si>
 </sst>
 </file>
@@ -111,10 +161,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3281EE86-C4A9-4434-A92F-ECAD45A4D158}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -449,7 +504,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -463,19 +518,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+    <row r="5" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>